<commit_message>
Add updated data dictionary, database manual, and upload template files to /public. Update home and upload controller actions to point to new downloadables.
</commit_message>
<xml_diff>
--- a/public/UploadResources/HLA_COVID19_data_dictionary_03262021.xlsx
+++ b/public/UploadResources/HLA_COVID19_data_dictionary_03262021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arenschen/DEV_REPOS/hlacovid_rails/hlacovid19/public/UploadResources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF2AB43E-2C96-7641-8CD1-5876ADEA1320}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474DFA30-F133-924A-8635-EC9BEF1E669C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50700" yWindow="-4420" windowWidth="41600" windowHeight="26660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <definedName name="comorbs5" localSheetId="0">Sheet1!$B$143:$C$172</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="222">
   <si>
     <t>column name</t>
   </si>
@@ -683,6 +682,27 @@
   </si>
   <si>
     <t>type_of_c19_test</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>authors</t>
+  </si>
+  <si>
+    <t>text (comma or semicolon delimited list)</t>
+  </si>
+  <si>
+    <t>pub_date</t>
+  </si>
+  <si>
+    <t>date (YYYY-MM-DD)</t>
+  </si>
+  <si>
+    <t>Publication</t>
   </si>
 </sst>
 </file>
@@ -745,7 +765,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -809,6 +829,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -891,7 +917,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -908,6 +934,25 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -925,9 +970,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -940,21 +982,15 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1178,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="B173" sqref="B173:B184"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="A185" sqref="A185:A188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1207,7 +1243,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="25" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1224,7 +1260,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="8" t="s">
         <v>198</v>
       </c>
@@ -1237,7 +1273,7 @@
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
@@ -1249,7 +1285,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1261,7 +1297,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1273,7 +1309,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="23"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1285,7 +1321,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="23"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1297,7 +1333,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
@@ -1312,7 +1348,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
@@ -1327,7 +1363,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
@@ -1342,7 +1378,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
@@ -1354,7 +1390,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="23"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
@@ -1365,86 +1401,86 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="23"/>
-      <c r="B14" s="34" t="s">
+    <row r="14" spans="1:11" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="25"/>
+      <c r="B14" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
+      <c r="D14" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="23"/>
-      <c r="B15" s="34" t="s">
+      <c r="A15" s="25"/>
+      <c r="B15" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="C15" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
+      <c r="C15" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="38"/>
-      <c r="B16" s="37" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-    </row>
-    <row r="17" spans="1:11" s="35" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="24" t="s">
+      <c r="C16" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+    </row>
+    <row r="17" spans="1:11" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
+      <c r="C17" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="5" t="s">
         <v>26</v>
       </c>
@@ -1456,7 +1492,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="5" t="s">
         <v>27</v>
       </c>
@@ -1468,7 +1504,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="5" t="s">
         <v>28</v>
       </c>
@@ -1480,7 +1516,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="5" t="s">
         <v>29</v>
       </c>
@@ -1492,7 +1528,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="5" t="s">
         <v>30</v>
       </c>
@@ -1504,7 +1540,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
+      <c r="A23" s="31"/>
       <c r="B23" s="5" t="s">
         <v>31</v>
       </c>
@@ -1516,7 +1552,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
+      <c r="A24" s="31"/>
       <c r="B24" s="5" t="s">
         <v>32</v>
       </c>
@@ -1528,7 +1564,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="5" t="s">
         <v>33</v>
       </c>
@@ -1540,7 +1576,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="5" t="s">
         <v>34</v>
       </c>
@@ -1552,7 +1588,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
+      <c r="A27" s="31"/>
       <c r="B27" s="5" t="s">
         <v>35</v>
       </c>
@@ -1564,7 +1600,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="20"/>
+      <c r="A28" s="31"/>
       <c r="B28" s="5" t="s">
         <v>36</v>
       </c>
@@ -1576,7 +1612,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="20"/>
+      <c r="A29" s="31"/>
       <c r="B29" s="5" t="s">
         <v>37</v>
       </c>
@@ -1588,7 +1624,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="20"/>
+      <c r="A30" s="31"/>
       <c r="B30" s="5" t="s">
         <v>38</v>
       </c>
@@ -1600,7 +1636,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="20"/>
+      <c r="A31" s="31"/>
       <c r="B31" s="5" t="s">
         <v>39</v>
       </c>
@@ -1612,7 +1648,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="20"/>
+      <c r="A32" s="31"/>
       <c r="B32" s="5" t="s">
         <v>40</v>
       </c>
@@ -1624,7 +1660,7 @@
       </c>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="20"/>
+      <c r="A33" s="31"/>
       <c r="B33" s="5" t="s">
         <v>41</v>
       </c>
@@ -1639,7 +1675,7 @@
       </c>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="20"/>
+      <c r="A34" s="31"/>
       <c r="B34" s="5" t="s">
         <v>44</v>
       </c>
@@ -1654,7 +1690,7 @@
       </c>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="20"/>
+      <c r="A35" s="31"/>
       <c r="B35" s="5" t="s">
         <v>46</v>
       </c>
@@ -1669,7 +1705,7 @@
       </c>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="20"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="5" t="s">
         <v>48</v>
       </c>
@@ -1684,7 +1720,7 @@
       </c>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="20"/>
+      <c r="A37" s="31"/>
       <c r="B37" s="5" t="s">
         <v>50</v>
       </c>
@@ -1699,7 +1735,7 @@
       </c>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="20"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="5" t="s">
         <v>53</v>
       </c>
@@ -1714,7 +1750,7 @@
       </c>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="20"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="5" t="s">
         <v>55</v>
       </c>
@@ -1729,7 +1765,7 @@
       </c>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="20"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="5" t="s">
         <v>57</v>
       </c>
@@ -1744,7 +1780,7 @@
       </c>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="20"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="5" t="s">
         <v>58</v>
       </c>
@@ -1759,7 +1795,7 @@
       </c>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="21"/>
+      <c r="A42" s="32"/>
       <c r="B42" s="9" t="s">
         <v>60</v>
       </c>
@@ -1795,7 +1831,7 @@
       <c r="Z42" s="9"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B43" s="6" t="s">
@@ -1809,7 +1845,7 @@
       </c>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="20"/>
+      <c r="A44" s="31"/>
       <c r="B44" s="15" t="s">
         <v>214</v>
       </c>
@@ -1821,7 +1857,7 @@
       </c>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="20"/>
+      <c r="A45" s="31"/>
       <c r="B45" s="5" t="s">
         <v>65</v>
       </c>
@@ -1833,7 +1869,7 @@
       </c>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="20"/>
+      <c r="A46" s="31"/>
       <c r="B46" s="5" t="s">
         <v>66</v>
       </c>
@@ -1845,7 +1881,7 @@
       </c>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="20"/>
+      <c r="A47" s="31"/>
       <c r="B47" s="5" t="s">
         <v>67</v>
       </c>
@@ -1857,7 +1893,7 @@
       </c>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="20"/>
+      <c r="A48" s="31"/>
       <c r="B48" s="5" t="s">
         <v>68</v>
       </c>
@@ -1869,7 +1905,7 @@
       </c>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="20"/>
+      <c r="A49" s="31"/>
       <c r="B49" s="5" t="s">
         <v>69</v>
       </c>
@@ -1881,7 +1917,7 @@
       </c>
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="20"/>
+      <c r="A50" s="31"/>
       <c r="B50" s="5" t="s">
         <v>70</v>
       </c>
@@ -1893,7 +1929,7 @@
       </c>
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="20"/>
+      <c r="A51" s="31"/>
       <c r="B51" s="5" t="s">
         <v>71</v>
       </c>
@@ -1905,7 +1941,7 @@
       </c>
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="20"/>
+      <c r="A52" s="31"/>
       <c r="B52" s="5" t="s">
         <v>72</v>
       </c>
@@ -1917,7 +1953,7 @@
       </c>
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="20"/>
+      <c r="A53" s="31"/>
       <c r="B53" s="5" t="s">
         <v>73</v>
       </c>
@@ -1929,7 +1965,7 @@
       </c>
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="20"/>
+      <c r="A54" s="31"/>
       <c r="B54" s="5" t="s">
         <v>74</v>
       </c>
@@ -1941,7 +1977,7 @@
       </c>
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="20"/>
+      <c r="A55" s="31"/>
       <c r="B55" s="5" t="s">
         <v>75</v>
       </c>
@@ -1953,7 +1989,7 @@
       </c>
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="20"/>
+      <c r="A56" s="31"/>
       <c r="B56" s="5" t="s">
         <v>76</v>
       </c>
@@ -1965,7 +2001,7 @@
       </c>
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="20"/>
+      <c r="A57" s="31"/>
       <c r="B57" s="5" t="s">
         <v>77</v>
       </c>
@@ -1977,7 +2013,7 @@
       </c>
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="20"/>
+      <c r="A58" s="31"/>
       <c r="B58" s="5" t="s">
         <v>78</v>
       </c>
@@ -1989,7 +2025,7 @@
       </c>
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="20"/>
+      <c r="A59" s="31"/>
       <c r="B59" s="5" t="s">
         <v>79</v>
       </c>
@@ -2001,7 +2037,7 @@
       </c>
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="21"/>
+      <c r="A60" s="32"/>
       <c r="B60" s="9" t="s">
         <v>80</v>
       </c>
@@ -2035,7 +2071,7 @@
       <c r="Z60" s="9"/>
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="26" t="s">
+      <c r="A61" s="36" t="s">
         <v>81</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -2049,7 +2085,7 @@
       </c>
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="20"/>
+      <c r="A62" s="31"/>
       <c r="B62" s="5" t="s">
         <v>83</v>
       </c>
@@ -2061,7 +2097,7 @@
       </c>
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="20"/>
+      <c r="A63" s="31"/>
       <c r="B63" s="6" t="s">
         <v>84</v>
       </c>
@@ -2073,7 +2109,7 @@
       </c>
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="20"/>
+      <c r="A64" s="31"/>
       <c r="B64" s="5" t="s">
         <v>85</v>
       </c>
@@ -2085,7 +2121,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="20"/>
+      <c r="A65" s="31"/>
       <c r="B65" s="5" t="s">
         <v>86</v>
       </c>
@@ -2097,7 +2133,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="20"/>
+      <c r="A66" s="31"/>
       <c r="B66" s="5" t="s">
         <v>87</v>
       </c>
@@ -2109,7 +2145,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="20"/>
+      <c r="A67" s="31"/>
       <c r="B67" s="5" t="s">
         <v>88</v>
       </c>
@@ -2121,7 +2157,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="20"/>
+      <c r="A68" s="31"/>
       <c r="B68" s="5" t="s">
         <v>89</v>
       </c>
@@ -2133,7 +2169,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="20"/>
+      <c r="A69" s="31"/>
       <c r="B69" s="5" t="s">
         <v>90</v>
       </c>
@@ -2145,7 +2181,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="20"/>
+      <c r="A70" s="31"/>
       <c r="B70" s="5" t="s">
         <v>91</v>
       </c>
@@ -2157,7 +2193,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="20"/>
+      <c r="A71" s="31"/>
       <c r="B71" s="5" t="s">
         <v>92</v>
       </c>
@@ -2169,7 +2205,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="20"/>
+      <c r="A72" s="31"/>
       <c r="B72" s="5" t="s">
         <v>93</v>
       </c>
@@ -2181,7 +2217,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="20"/>
+      <c r="A73" s="31"/>
       <c r="B73" s="5" t="s">
         <v>94</v>
       </c>
@@ -2193,7 +2229,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="20"/>
+      <c r="A74" s="31"/>
       <c r="B74" s="5" t="s">
         <v>95</v>
       </c>
@@ -2205,7 +2241,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="20"/>
+      <c r="A75" s="31"/>
       <c r="B75" s="5" t="s">
         <v>96</v>
       </c>
@@ -2217,7 +2253,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="20"/>
+      <c r="A76" s="31"/>
       <c r="B76" s="5" t="s">
         <v>97</v>
       </c>
@@ -2229,7 +2265,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="20"/>
+      <c r="A77" s="31"/>
       <c r="B77" s="5" t="s">
         <v>98</v>
       </c>
@@ -2241,7 +2277,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="20"/>
+      <c r="A78" s="31"/>
       <c r="B78" s="5" t="s">
         <v>99</v>
       </c>
@@ -2253,7 +2289,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="20"/>
+      <c r="A79" s="31"/>
       <c r="B79" s="5" t="s">
         <v>100</v>
       </c>
@@ -2265,7 +2301,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="20"/>
+      <c r="A80" s="31"/>
       <c r="B80" s="5" t="s">
         <v>101</v>
       </c>
@@ -2277,7 +2313,7 @@
       </c>
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="20"/>
+      <c r="A81" s="31"/>
       <c r="B81" s="8" t="s">
         <v>199</v>
       </c>
@@ -2289,7 +2325,7 @@
       </c>
     </row>
     <row r="82" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="20"/>
+      <c r="A82" s="31"/>
       <c r="B82" s="5" t="s">
         <v>102</v>
       </c>
@@ -2301,7 +2337,7 @@
       </c>
     </row>
     <row r="83" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="20"/>
+      <c r="A83" s="31"/>
       <c r="B83" s="5" t="s">
         <v>103</v>
       </c>
@@ -2313,7 +2349,7 @@
       </c>
     </row>
     <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="20"/>
+      <c r="A84" s="31"/>
       <c r="B84" s="5" t="s">
         <v>104</v>
       </c>
@@ -2325,7 +2361,7 @@
       </c>
     </row>
     <row r="85" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="20"/>
+      <c r="A85" s="31"/>
       <c r="B85" s="5" t="s">
         <v>105</v>
       </c>
@@ -2337,7 +2373,7 @@
       </c>
     </row>
     <row r="86" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="20"/>
+      <c r="A86" s="31"/>
       <c r="B86" s="5" t="s">
         <v>106</v>
       </c>
@@ -2349,7 +2385,7 @@
       </c>
     </row>
     <row r="87" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="21"/>
+      <c r="A87" s="32"/>
       <c r="B87" s="9" t="s">
         <v>107</v>
       </c>
@@ -2383,7 +2419,7 @@
       <c r="Z87" s="9"/>
     </row>
     <row r="88" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="27" t="s">
+      <c r="A88" s="37" t="s">
         <v>108</v>
       </c>
       <c r="B88" s="6" t="s">
@@ -2397,7 +2433,7 @@
       </c>
     </row>
     <row r="89" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="20"/>
+      <c r="A89" s="31"/>
       <c r="B89" s="5" t="s">
         <v>110</v>
       </c>
@@ -2409,7 +2445,7 @@
       </c>
     </row>
     <row r="90" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="20"/>
+      <c r="A90" s="31"/>
       <c r="B90" s="5" t="s">
         <v>111</v>
       </c>
@@ -2421,7 +2457,7 @@
       </c>
     </row>
     <row r="91" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="21"/>
+      <c r="A91" s="32"/>
       <c r="B91" s="9" t="s">
         <v>112</v>
       </c>
@@ -2455,7 +2491,7 @@
       <c r="Z91" s="9"/>
     </row>
     <row r="92" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="19" t="s">
+      <c r="A92" s="30" t="s">
         <v>113</v>
       </c>
       <c r="B92" s="5" t="s">
@@ -2469,7 +2505,7 @@
       </c>
     </row>
     <row r="93" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="20"/>
+      <c r="A93" s="31"/>
       <c r="B93" s="5" t="s">
         <v>115</v>
       </c>
@@ -2481,7 +2517,7 @@
       </c>
     </row>
     <row r="94" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="20"/>
+      <c r="A94" s="31"/>
       <c r="B94" s="5" t="s">
         <v>116</v>
       </c>
@@ -2493,7 +2529,7 @@
       </c>
     </row>
     <row r="95" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="20"/>
+      <c r="A95" s="31"/>
       <c r="B95" s="5" t="s">
         <v>117</v>
       </c>
@@ -2505,7 +2541,7 @@
       </c>
     </row>
     <row r="96" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="20"/>
+      <c r="A96" s="31"/>
       <c r="B96" s="5" t="s">
         <v>118</v>
       </c>
@@ -2517,7 +2553,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="20"/>
+      <c r="A97" s="31"/>
       <c r="B97" s="5" t="s">
         <v>119</v>
       </c>
@@ -2529,7 +2565,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="20"/>
+      <c r="A98" s="31"/>
       <c r="B98" s="5" t="s">
         <v>120</v>
       </c>
@@ -2541,7 +2577,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="20"/>
+      <c r="A99" s="31"/>
       <c r="B99" s="5" t="s">
         <v>121</v>
       </c>
@@ -2553,7 +2589,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="20"/>
+      <c r="A100" s="31"/>
       <c r="B100" s="5" t="s">
         <v>122</v>
       </c>
@@ -2565,7 +2601,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="20"/>
+      <c r="A101" s="31"/>
       <c r="B101" s="5" t="s">
         <v>123</v>
       </c>
@@ -2577,7 +2613,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="20"/>
+      <c r="A102" s="31"/>
       <c r="B102" s="5" t="s">
         <v>124</v>
       </c>
@@ -2589,7 +2625,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="20"/>
+      <c r="A103" s="31"/>
       <c r="B103" s="5" t="s">
         <v>125</v>
       </c>
@@ -2601,7 +2637,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="20"/>
+      <c r="A104" s="31"/>
       <c r="B104" s="5" t="s">
         <v>126</v>
       </c>
@@ -2613,7 +2649,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="20"/>
+      <c r="A105" s="31"/>
       <c r="B105" s="5" t="s">
         <v>127</v>
       </c>
@@ -2625,7 +2661,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="20"/>
+      <c r="A106" s="31"/>
       <c r="B106" s="5" t="s">
         <v>128</v>
       </c>
@@ -2637,7 +2673,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="20"/>
+      <c r="A107" s="31"/>
       <c r="B107" s="5" t="s">
         <v>129</v>
       </c>
@@ -2649,7 +2685,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="20"/>
+      <c r="A108" s="31"/>
       <c r="B108" s="5" t="s">
         <v>130</v>
       </c>
@@ -2661,7 +2697,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="20"/>
+      <c r="A109" s="31"/>
       <c r="B109" s="5" t="s">
         <v>131</v>
       </c>
@@ -2673,7 +2709,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="20"/>
+      <c r="A110" s="31"/>
       <c r="B110" s="5" t="s">
         <v>132</v>
       </c>
@@ -2685,7 +2721,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="20"/>
+      <c r="A111" s="31"/>
       <c r="B111" s="5" t="s">
         <v>133</v>
       </c>
@@ -2697,7 +2733,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="20"/>
+      <c r="A112" s="31"/>
       <c r="B112" s="5" t="s">
         <v>134</v>
       </c>
@@ -2709,7 +2745,7 @@
       </c>
     </row>
     <row r="113" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="20"/>
+      <c r="A113" s="31"/>
       <c r="B113" s="5" t="s">
         <v>135</v>
       </c>
@@ -2721,7 +2757,7 @@
       </c>
     </row>
     <row r="114" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="20"/>
+      <c r="A114" s="31"/>
       <c r="B114" s="5" t="s">
         <v>136</v>
       </c>
@@ -2733,7 +2769,7 @@
       </c>
     </row>
     <row r="115" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="20"/>
+      <c r="A115" s="31"/>
       <c r="B115" s="5" t="s">
         <v>137</v>
       </c>
@@ -2745,7 +2781,7 @@
       </c>
     </row>
     <row r="116" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="20"/>
+      <c r="A116" s="31"/>
       <c r="B116" s="5" t="s">
         <v>138</v>
       </c>
@@ -2757,7 +2793,7 @@
       </c>
     </row>
     <row r="117" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="20"/>
+      <c r="A117" s="31"/>
       <c r="B117" s="5" t="s">
         <v>139</v>
       </c>
@@ -2769,7 +2805,7 @@
       </c>
     </row>
     <row r="118" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="20"/>
+      <c r="A118" s="31"/>
       <c r="B118" s="5" t="s">
         <v>140</v>
       </c>
@@ -2781,7 +2817,7 @@
       </c>
     </row>
     <row r="119" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="20"/>
+      <c r="A119" s="31"/>
       <c r="B119" s="5" t="s">
         <v>141</v>
       </c>
@@ -2793,7 +2829,7 @@
       </c>
     </row>
     <row r="120" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="20"/>
+      <c r="A120" s="31"/>
       <c r="B120" s="5" t="s">
         <v>142</v>
       </c>
@@ -2805,7 +2841,7 @@
       </c>
     </row>
     <row r="121" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="20"/>
+      <c r="A121" s="31"/>
       <c r="B121" s="5" t="s">
         <v>143</v>
       </c>
@@ -2817,7 +2853,7 @@
       </c>
     </row>
     <row r="122" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="20"/>
+      <c r="A122" s="31"/>
       <c r="B122" s="5" t="s">
         <v>144</v>
       </c>
@@ -2829,7 +2865,7 @@
       </c>
     </row>
     <row r="123" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="20"/>
+      <c r="A123" s="31"/>
       <c r="B123" s="5" t="s">
         <v>145</v>
       </c>
@@ -2841,7 +2877,7 @@
       </c>
     </row>
     <row r="124" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="20"/>
+      <c r="A124" s="31"/>
       <c r="B124" s="5" t="s">
         <v>146</v>
       </c>
@@ -2853,7 +2889,7 @@
       </c>
     </row>
     <row r="125" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="21"/>
+      <c r="A125" s="32"/>
       <c r="B125" s="9" t="s">
         <v>147</v>
       </c>
@@ -2887,7 +2923,7 @@
       <c r="Z125" s="9"/>
     </row>
     <row r="126" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="22" t="s">
+      <c r="A126" s="33" t="s">
         <v>148</v>
       </c>
       <c r="B126" s="5" t="s">
@@ -2901,7 +2937,7 @@
       </c>
     </row>
     <row r="127" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="20"/>
+      <c r="A127" s="31"/>
       <c r="B127" s="5" t="s">
         <v>150</v>
       </c>
@@ -2913,7 +2949,7 @@
       </c>
     </row>
     <row r="128" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="20"/>
+      <c r="A128" s="31"/>
       <c r="B128" s="5" t="s">
         <v>151</v>
       </c>
@@ -2925,7 +2961,7 @@
       </c>
     </row>
     <row r="129" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="20"/>
+      <c r="A129" s="31"/>
       <c r="B129" s="5" t="s">
         <v>152</v>
       </c>
@@ -2937,7 +2973,7 @@
       </c>
     </row>
     <row r="130" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="20"/>
+      <c r="A130" s="31"/>
       <c r="B130" s="5" t="s">
         <v>153</v>
       </c>
@@ -2949,7 +2985,7 @@
       </c>
     </row>
     <row r="131" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="20"/>
+      <c r="A131" s="31"/>
       <c r="B131" s="5" t="s">
         <v>154</v>
       </c>
@@ -2961,7 +2997,7 @@
       </c>
     </row>
     <row r="132" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="20"/>
+      <c r="A132" s="31"/>
       <c r="B132" s="5" t="s">
         <v>155</v>
       </c>
@@ -2973,7 +3009,7 @@
       </c>
     </row>
     <row r="133" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="20"/>
+      <c r="A133" s="31"/>
       <c r="B133" s="5" t="s">
         <v>156</v>
       </c>
@@ -2985,7 +3021,7 @@
       </c>
     </row>
     <row r="134" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="20"/>
+      <c r="A134" s="31"/>
       <c r="B134" s="5" t="s">
         <v>157</v>
       </c>
@@ -2997,7 +3033,7 @@
       </c>
     </row>
     <row r="135" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="20"/>
+      <c r="A135" s="31"/>
       <c r="B135" s="5" t="s">
         <v>158</v>
       </c>
@@ -3009,7 +3045,7 @@
       </c>
     </row>
     <row r="136" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="20"/>
+      <c r="A136" s="31"/>
       <c r="B136" s="5" t="s">
         <v>159</v>
       </c>
@@ -3021,7 +3057,7 @@
       </c>
     </row>
     <row r="137" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="20"/>
+      <c r="A137" s="31"/>
       <c r="B137" s="5" t="s">
         <v>160</v>
       </c>
@@ -3033,7 +3069,7 @@
       </c>
     </row>
     <row r="138" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="20"/>
+      <c r="A138" s="31"/>
       <c r="B138" s="5" t="s">
         <v>161</v>
       </c>
@@ -3045,7 +3081,7 @@
       </c>
     </row>
     <row r="139" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="20"/>
+      <c r="A139" s="31"/>
       <c r="B139" s="5" t="s">
         <v>162</v>
       </c>
@@ -3057,7 +3093,7 @@
       </c>
     </row>
     <row r="140" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="20"/>
+      <c r="A140" s="31"/>
       <c r="B140" s="5" t="s">
         <v>163</v>
       </c>
@@ -3069,7 +3105,7 @@
       </c>
     </row>
     <row r="141" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="20"/>
+      <c r="A141" s="31"/>
       <c r="B141" s="5" t="s">
         <v>164</v>
       </c>
@@ -3081,7 +3117,7 @@
       </c>
     </row>
     <row r="142" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="21"/>
+      <c r="A142" s="32"/>
       <c r="B142" s="9" t="s">
         <v>165</v>
       </c>
@@ -3115,7 +3151,7 @@
       <c r="Z142" s="9"/>
     </row>
     <row r="143" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A143" s="16" t="s">
+      <c r="A143" s="27" t="s">
         <v>197</v>
       </c>
       <c r="B143" s="12" t="s">
@@ -3129,7 +3165,7 @@
       </c>
     </row>
     <row r="144" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A144" s="17"/>
+      <c r="A144" s="28"/>
       <c r="B144" s="12" t="s">
         <v>167</v>
       </c>
@@ -3141,7 +3177,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A145" s="17"/>
+      <c r="A145" s="28"/>
       <c r="B145" s="12" t="s">
         <v>169</v>
       </c>
@@ -3153,7 +3189,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A146" s="17"/>
+      <c r="A146" s="28"/>
       <c r="B146" s="12" t="s">
         <v>170</v>
       </c>
@@ -3165,7 +3201,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A147" s="17"/>
+      <c r="A147" s="28"/>
       <c r="B147" s="12" t="s">
         <v>171</v>
       </c>
@@ -3177,7 +3213,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A148" s="17"/>
+      <c r="A148" s="28"/>
       <c r="B148" s="12" t="s">
         <v>172</v>
       </c>
@@ -3189,7 +3225,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A149" s="17"/>
+      <c r="A149" s="28"/>
       <c r="B149" s="12" t="s">
         <v>173</v>
       </c>
@@ -3201,7 +3237,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A150" s="17"/>
+      <c r="A150" s="28"/>
       <c r="B150" s="12" t="s">
         <v>174</v>
       </c>
@@ -3213,7 +3249,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A151" s="17"/>
+      <c r="A151" s="28"/>
       <c r="B151" s="12" t="s">
         <v>175</v>
       </c>
@@ -3225,7 +3261,7 @@
       </c>
     </row>
     <row r="152" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A152" s="17"/>
+      <c r="A152" s="28"/>
       <c r="B152" s="12" t="s">
         <v>176</v>
       </c>
@@ -3237,7 +3273,7 @@
       </c>
     </row>
     <row r="153" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A153" s="17"/>
+      <c r="A153" s="28"/>
       <c r="B153" s="12" t="s">
         <v>177</v>
       </c>
@@ -3249,7 +3285,7 @@
       </c>
     </row>
     <row r="154" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A154" s="17"/>
+      <c r="A154" s="28"/>
       <c r="B154" s="12" t="s">
         <v>178</v>
       </c>
@@ -3261,7 +3297,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A155" s="17"/>
+      <c r="A155" s="28"/>
       <c r="B155" s="12" t="s">
         <v>179</v>
       </c>
@@ -3273,7 +3309,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A156" s="17"/>
+      <c r="A156" s="28"/>
       <c r="B156" s="12" t="s">
         <v>180</v>
       </c>
@@ -3285,7 +3321,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A157" s="17"/>
+      <c r="A157" s="28"/>
       <c r="B157" s="12" t="s">
         <v>181</v>
       </c>
@@ -3297,7 +3333,7 @@
       </c>
     </row>
     <row r="158" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A158" s="17"/>
+      <c r="A158" s="28"/>
       <c r="B158" s="12" t="s">
         <v>182</v>
       </c>
@@ -3309,7 +3345,7 @@
       </c>
     </row>
     <row r="159" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A159" s="17"/>
+      <c r="A159" s="28"/>
       <c r="B159" s="12" t="s">
         <v>183</v>
       </c>
@@ -3321,7 +3357,7 @@
       </c>
     </row>
     <row r="160" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A160" s="17"/>
+      <c r="A160" s="28"/>
       <c r="B160" s="12" t="s">
         <v>184</v>
       </c>
@@ -3333,7 +3369,7 @@
       </c>
     </row>
     <row r="161" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A161" s="17"/>
+      <c r="A161" s="28"/>
       <c r="B161" s="12" t="s">
         <v>185</v>
       </c>
@@ -3345,7 +3381,7 @@
       </c>
     </row>
     <row r="162" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A162" s="17"/>
+      <c r="A162" s="28"/>
       <c r="B162" s="12" t="s">
         <v>186</v>
       </c>
@@ -3357,7 +3393,7 @@
       </c>
     </row>
     <row r="163" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A163" s="17"/>
+      <c r="A163" s="28"/>
       <c r="B163" s="12" t="s">
         <v>187</v>
       </c>
@@ -3369,7 +3405,7 @@
       </c>
     </row>
     <row r="164" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A164" s="17"/>
+      <c r="A164" s="28"/>
       <c r="B164" s="12" t="s">
         <v>188</v>
       </c>
@@ -3381,7 +3417,7 @@
       </c>
     </row>
     <row r="165" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A165" s="17"/>
+      <c r="A165" s="28"/>
       <c r="B165" s="12" t="s">
         <v>189</v>
       </c>
@@ -3393,7 +3429,7 @@
       </c>
     </row>
     <row r="166" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A166" s="17"/>
+      <c r="A166" s="28"/>
       <c r="B166" s="12" t="s">
         <v>190</v>
       </c>
@@ -3405,7 +3441,7 @@
       </c>
     </row>
     <row r="167" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A167" s="17"/>
+      <c r="A167" s="28"/>
       <c r="B167" s="12" t="s">
         <v>191</v>
       </c>
@@ -3417,7 +3453,7 @@
       </c>
     </row>
     <row r="168" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A168" s="17"/>
+      <c r="A168" s="28"/>
       <c r="B168" s="12" t="s">
         <v>192</v>
       </c>
@@ -3429,7 +3465,7 @@
       </c>
     </row>
     <row r="169" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A169" s="17"/>
+      <c r="A169" s="28"/>
       <c r="B169" s="12" t="s">
         <v>193</v>
       </c>
@@ -3441,7 +3477,7 @@
       </c>
     </row>
     <row r="170" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A170" s="17"/>
+      <c r="A170" s="28"/>
       <c r="B170" s="12" t="s">
         <v>194</v>
       </c>
@@ -3453,7 +3489,7 @@
       </c>
     </row>
     <row r="171" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A171" s="17"/>
+      <c r="A171" s="28"/>
       <c r="B171" s="12" t="s">
         <v>195</v>
       </c>
@@ -3465,25 +3501,25 @@
       </c>
     </row>
     <row r="172" spans="1:4" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A172" s="18"/>
+      <c r="A172" s="29"/>
       <c r="B172" s="13" t="s">
         <v>196</v>
       </c>
       <c r="C172" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D172" s="33" t="s">
+      <c r="D172" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="29" t="s">
+      <c r="A173" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="B173" s="28" t="s">
+      <c r="B173" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="C173" s="28" t="s">
+      <c r="C173" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D173" t="s">
@@ -3491,11 +3527,11 @@
       </c>
     </row>
     <row r="174" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="30"/>
-      <c r="B174" s="28" t="s">
+      <c r="A174" s="24"/>
+      <c r="B174" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="C174" s="28" t="s">
+      <c r="C174" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D174" t="s">
@@ -3503,11 +3539,11 @@
       </c>
     </row>
     <row r="175" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="30"/>
-      <c r="B175" s="28" t="s">
+      <c r="A175" s="24"/>
+      <c r="B175" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="C175" s="28" t="s">
+      <c r="C175" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D175" t="s">
@@ -3515,11 +3551,11 @@
       </c>
     </row>
     <row r="176" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="30"/>
-      <c r="B176" s="28" t="s">
+      <c r="A176" s="24"/>
+      <c r="B176" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="C176" s="28" t="s">
+      <c r="C176" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D176" t="s">
@@ -3527,11 +3563,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="30"/>
-      <c r="B177" s="28" t="s">
+      <c r="A177" s="24"/>
+      <c r="B177" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="C177" s="28" t="s">
+      <c r="C177" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D177" t="s">
@@ -3539,11 +3575,11 @@
       </c>
     </row>
     <row r="178" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="30"/>
-      <c r="B178" s="28" t="s">
+      <c r="A178" s="24"/>
+      <c r="B178" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="C178" s="28" t="s">
+      <c r="C178" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D178" t="s">
@@ -3551,11 +3587,11 @@
       </c>
     </row>
     <row r="179" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A179" s="30"/>
-      <c r="B179" s="28" t="s">
+      <c r="A179" s="24"/>
+      <c r="B179" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="C179" s="28" t="s">
+      <c r="C179" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D179" t="s">
@@ -3563,11 +3599,11 @@
       </c>
     </row>
     <row r="180" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A180" s="30"/>
-      <c r="B180" s="28" t="s">
+      <c r="A180" s="24"/>
+      <c r="B180" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="C180" s="28" t="s">
+      <c r="C180" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D180" t="s">
@@ -3575,11 +3611,11 @@
       </c>
     </row>
     <row r="181" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A181" s="30"/>
-      <c r="B181" s="28" t="s">
+      <c r="A181" s="24"/>
+      <c r="B181" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="C181" s="28" t="s">
+      <c r="C181" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D181" t="s">
@@ -3587,11 +3623,11 @@
       </c>
     </row>
     <row r="182" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A182" s="30"/>
-      <c r="B182" s="28" t="s">
+      <c r="A182" s="24"/>
+      <c r="B182" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="C182" s="28" t="s">
+      <c r="C182" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D182" t="s">
@@ -3599,11 +3635,11 @@
       </c>
     </row>
     <row r="183" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A183" s="30"/>
-      <c r="B183" s="28" t="s">
+      <c r="A183" s="24"/>
+      <c r="B183" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="C183" s="28" t="s">
+      <c r="C183" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D183" t="s">
@@ -3611,11 +3647,11 @@
       </c>
     </row>
     <row r="184" spans="1:4" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A184" s="30"/>
-      <c r="B184" s="31" t="s">
+      <c r="A184" s="24"/>
+      <c r="B184" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="C184" s="31" t="s">
+      <c r="C184" s="17" t="s">
         <v>6</v>
       </c>
       <c r="D184" s="14" t="s">
@@ -3623,11 +3659,55 @@
       </c>
     </row>
     <row r="185" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A185" s="32"/>
-    </row>
-    <row r="186" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="187" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="188" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="A185" s="39" t="s">
+        <v>221</v>
+      </c>
+      <c r="B185" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="C185" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D185" s="38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="40"/>
+      <c r="B186" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="C186" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D186" s="38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A187" s="40"/>
+      <c r="B187" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="C187" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="D187" s="38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="42"/>
+      <c r="B188" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="C188" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="D188" s="41" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="189" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="190" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="191" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4443,7 +4523,8 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A185:A188"/>
     <mergeCell ref="A173:A184"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A143:A172"/>

</xml_diff>